<commit_message>
Update: Doing Code SS5
</commit_message>
<xml_diff>
--- a/Docs/Cornell Note_SpringBoot.xlsx
+++ b/Docs/Cornell Note_SpringBoot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Common\A1221I1_HuynhKimSon\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeGym\A1221I1_HuynhKimSon\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DA8499-B321-41C4-B6FF-9793AB6951E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A990C4-8349-4810-859D-91FA5E4B0113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="495" windowWidth="28770" windowHeight="15255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SS1_1" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>STT</t>
   </si>
@@ -55,9 +55,6 @@
     <t>REST nó sd kiểu dữ liệu JSON để tương tác</t>
   </si>
   <si>
-    <t>hiểu đơn giản là biến 1 java class thông thường thành API trong restful web service</t>
-  </si>
-  <si>
     <t>@RequestMapping</t>
   </si>
   <si>
@@ -65,15 +62,6 @@
   </si>
   <si>
     <t>@Controller</t>
-  </si>
-  <si>
-    <t>nhận resquest từ client vào</t>
-  </si>
-  <si>
-    <t>RequestMethod.Post</t>
-  </si>
-  <si>
-    <t>kiểu HTTP method, POST được dùng trong các trường hợp chúng ta thêm dữ liệu vào trong db</t>
   </si>
   <si>
     <t>nhận dữ liệu json được truyền từ client vào server</t>
@@ -94,10 +82,6 @@
 - hiển thị dữ liệu : GET</t>
   </si>
   <si>
-    <t>@RestController thay thế cho @Controller + @ResponseBody
-@PostMapping thay thế cho @RequestMapping + RequestMethod.POST</t>
-  </si>
-  <si>
     <t>@RequestParam</t>
   </si>
   <si>
@@ -107,18 +91,37 @@
     <t>@Autowire</t>
   </si>
   <si>
-    <t>- được sử dụng để xử lý những URL động, có một hoặc nhiều parameter trong URL.
-Ví dụ bên dưới khi người dùng gõ vào là http://localhost:8080/test2/10/nguyen.
-test2: sẽ ứng với method test2 trong controller thông qua @Request.
-10: số 10 sẽ được gán vào biên id nhờ PathVariable (@PathVariable(“id”) int id).
-nguyen: chữ nguyên sẽ gán vào biến name nhờ PathVariable (@PathVariable(“name”) String name).</t>
-  </si>
-  <si>
-    <t>- để bắt các giá trị các tham số mà người dùng truyền vào trên URL theo định dạng key và value.
-Ví dụ tôi có cái link sau http://localhost:8080/api/foos?id=abc. 
-muốn lấy giá trị abc của tham số id trên URL thì tôi sẽ dùng @RequestParam. Ở đây  khai báo giá trị tham số trên URL theo định dạng key = value (id=abc).
-Chúng ta khai báo @RequestParame trong method getFoos(@RequestParam String id). 
-Như vậy biến id sẽ có giá trị là abc nhờ cơ chế mapping.</t>
+    <t>Lấy giá trị trên url theo định dang key-value (param động)</t>
+  </si>
+  <si>
+    <t>Lấy giá trị tham số tĩnh trên url, có thể sd regex</t>
+  </si>
+  <si>
+    <t>Thực hiện DI dependency injection tìm tới bean khai báo</t>
+  </si>
+  <si>
+    <t>@GetMapping, @PostMapping</t>
+  </si>
+  <si>
+    <t>đón nhận http get, post</t>
+  </si>
+  <si>
+    <t>ánh xạ resquest từ client gửi lên</t>
+  </si>
+  <si>
+    <t>dùng để đánh dấu một class là spring MVC controller dùng cho web application</t>
+  </si>
+  <si>
+    <t>@RestController</t>
+  </si>
+  <si>
+    <t>dùng để đánh dấu một class là restful controller dùng cho web-service</t>
+  </si>
+  <si>
+    <t>@ModelAttribute</t>
+  </si>
+  <si>
+    <t>để liên kết các tham số yêu cầu hoặc các trường form với một đối tượng</t>
   </si>
 </sst>
 </file>
@@ -211,11 +214,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -497,30 +500,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4D174D-7D86-4A0E-AD79-E65C83EF958B}">
-  <dimension ref="B1:D29"/>
+  <dimension ref="B1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="88.28515625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="2.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="88.33203125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+    <row r="1" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-    </row>
-    <row r="3" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -531,7 +534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5">
         <v>1</v>
       </c>
@@ -542,7 +545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5">
         <v>2</v>
       </c>
@@ -551,207 +554,222 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>10</v>
+      <c r="C6" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>8</v>
+      <c r="C7" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>12</v>
+      <c r="C8" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5">
         <v>6</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>9</v>
+      <c r="C9" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="112.15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="D10" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="112.15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="112.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5">
         <v>8</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>15</v>
-      </c>
+      <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="112.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="5">
         <v>9</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="5">
         <v>10</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="5">
         <v>11</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="5">
         <v>12</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="5">
         <v>13</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5">
         <v>14</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="5">
         <v>15</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="5">
         <v>16</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="5">
         <v>17</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="5">
         <v>18</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="5">
         <v>19</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="5">
         <v>20</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="5">
         <v>21</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="5">
         <v>22</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5">
         <v>23</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="5">
         <v>24</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="5">
         <v>25</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="5">
         <v>26</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="5">
+        <v>27</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>